<commit_message>
fix tanggal kejadian ACO Map
</commit_message>
<xml_diff>
--- a/output/aco_results/aco_zoning_data_for_lstm.xlsx
+++ b/output/aco_results/aco_zoning_data_for_lstm.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -486,7 +490,9 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
+      <c r="A2" s="2" t="n">
+        <v>46003.14027777778</v>
+      </c>
       <c r="B2" t="n">
         <v>-8</v>
       </c>
@@ -516,7 +522,9 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
+      <c r="A3" s="2" t="n">
+        <v>46003.14027777778</v>
+      </c>
       <c r="B3" t="n">
         <v>-8</v>
       </c>
@@ -546,7 +554,9 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
+      <c r="A4" s="2" t="n">
+        <v>46003.23680555556</v>
+      </c>
       <c r="B4" t="n">
         <v>-7.97</v>
       </c>
@@ -576,7 +586,9 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
+      <c r="A5" s="2" t="n">
+        <v>46003.76111111111</v>
+      </c>
       <c r="B5" t="n">
         <v>-7.91</v>
       </c>
@@ -606,7 +618,9 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
+      <c r="A6" s="2" t="n">
+        <v>46004.62708333333</v>
+      </c>
       <c r="B6" t="n">
         <v>-7.98</v>
       </c>
@@ -636,7 +650,9 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" s="2" t="n">
+        <v>46004.99583333333</v>
+      </c>
       <c r="B7" t="n">
         <v>-7.97</v>
       </c>
@@ -666,7 +682,9 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
+      <c r="A8" s="2" t="n">
+        <v>46006.00833333333</v>
+      </c>
       <c r="B8" t="n">
         <v>-7.97</v>
       </c>
@@ -696,7 +714,9 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" s="2" t="n">
+        <v>46006.48263888889</v>
+      </c>
       <c r="B9" t="n">
         <v>-7.99</v>
       </c>
@@ -726,7 +746,9 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr"/>
+      <c r="A10" s="2" t="n">
+        <v>46006.86041666667</v>
+      </c>
       <c r="B10" t="n">
         <v>-7.96</v>
       </c>

</xml_diff>

<commit_message>
fix rmv vs aoc, but failed rmv roc_aoc
</commit_message>
<xml_diff>
--- a/output/aco_results/aco_zoning_data_for_lstm.xlsx
+++ b/output/aco_results/aco_zoning_data_for_lstm.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,90 +491,90 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46003.14027777778</v>
+        <v>46000.94930555556</v>
       </c>
       <c r="B2" t="n">
-        <v>-8</v>
+        <v>-8.01</v>
       </c>
       <c r="C2" t="n">
-        <v>114.19</v>
+        <v>114.18</v>
       </c>
       <c r="D2" t="n">
-        <v>2.1</v>
+        <v>2.9</v>
       </c>
       <c r="E2" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="n">
-        <v>0.5</v>
+        <v>0.9450121840697095</v>
       </c>
       <c r="H2" t="n">
-        <v>50</v>
+        <v>94.5</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Aman</t>
+          <t>Terdampak</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>3.279405314694293</v>
+        <v>5.877254504294055</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46003.14027777778</v>
+        <v>46000.94930555556</v>
       </c>
       <c r="B3" t="n">
-        <v>-8</v>
+        <v>-8.01</v>
       </c>
       <c r="C3" t="n">
-        <v>114.19</v>
+        <v>114.18</v>
       </c>
       <c r="D3" t="n">
-        <v>2.1</v>
+        <v>2.9</v>
       </c>
       <c r="E3" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
-        <v>0.5</v>
+        <v>0.9511983133618672</v>
       </c>
       <c r="H3" t="n">
-        <v>50</v>
+        <v>95.12</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Aman</t>
+          <t>Terdampak</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>3.279405314694293</v>
+        <v>5.88959993921047</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>46003.23680555556</v>
+        <v>46000.96944444445</v>
       </c>
       <c r="B4" t="n">
-        <v>-7.97</v>
+        <v>-7.96</v>
       </c>
       <c r="C4" t="n">
-        <v>114.13</v>
+        <v>112.77</v>
       </c>
       <c r="D4" t="n">
-        <v>2.2</v>
+        <v>2.1</v>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="n">
-        <v>0.5</v>
+        <v>0.0001</v>
       </c>
       <c r="H4" t="n">
-        <v>50</v>
+        <v>0.01</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -582,31 +582,31 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>3.483850403030317</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46003.76111111111</v>
+        <v>46000.96944444445</v>
       </c>
       <c r="B5" t="n">
-        <v>-7.91</v>
+        <v>-7.96</v>
       </c>
       <c r="C5" t="n">
-        <v>114.14</v>
+        <v>112.77</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="E5" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="n">
-        <v>0.5</v>
+        <v>0.05978295139323081</v>
       </c>
       <c r="H5" t="n">
-        <v>50</v>
+        <v>5.98</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -614,167 +614,551 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>3.077861033362291</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>46004.62708333333</v>
+        <v>46002.14027777778</v>
       </c>
       <c r="B6" t="n">
         <v>-7.98</v>
       </c>
       <c r="C6" t="n">
-        <v>114.24</v>
+        <v>114.15</v>
       </c>
       <c r="D6" t="n">
-        <v>3.1</v>
+        <v>2.2</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="n">
-        <v>0.5</v>
+        <v>0.8662135250639107</v>
       </c>
       <c r="H6" t="n">
-        <v>50</v>
+        <v>86.62</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Aman</t>
+          <t>Terdampak</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>5.441018655854489</v>
+        <v>3.99418365778594</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>46004.99583333333</v>
+        <v>46002.14027777778</v>
       </c>
       <c r="B7" t="n">
-        <v>-7.97</v>
+        <v>-7.98</v>
       </c>
       <c r="C7" t="n">
-        <v>114.16</v>
+        <v>114.15</v>
       </c>
       <c r="D7" t="n">
-        <v>2.3</v>
+        <v>2.2</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="n">
-        <v>0.5</v>
+        <v>0.7810637733539998</v>
       </c>
       <c r="H7" t="n">
-        <v>50</v>
+        <v>78.11</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Aman</t>
+          <t>Terdampak</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>3.691103301765151</v>
+        <v>3.875524059060939</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>46006.00833333333</v>
+        <v>46002.91805555556</v>
       </c>
       <c r="B8" t="n">
-        <v>-7.97</v>
+        <v>-7.92</v>
       </c>
       <c r="C8" t="n">
-        <v>114.15</v>
+        <v>114.16</v>
       </c>
       <c r="D8" t="n">
         <v>2.2</v>
       </c>
       <c r="E8" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="n">
-        <v>0.5</v>
+        <v>0.9175182761045644</v>
       </c>
       <c r="H8" t="n">
-        <v>50</v>
+        <v>91.75</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Aman</t>
+          <t>Terdampak</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>3.483850403030317</v>
+        <v>4.065678888822081</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>46006.48263888889</v>
+        <v>46002.91805555556</v>
       </c>
       <c r="B9" t="n">
-        <v>-7.99</v>
+        <v>-7.92</v>
       </c>
       <c r="C9" t="n">
-        <v>114.19</v>
+        <v>114.16</v>
       </c>
       <c r="D9" t="n">
-        <v>2.6</v>
+        <v>2.2</v>
       </c>
       <c r="E9" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="n">
-        <v>0.5</v>
+        <v>0.8796969689600115</v>
       </c>
       <c r="H9" t="n">
-        <v>50</v>
+        <v>87.97</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Aman</t>
+          <t>Terdampak</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>4.328878189671251</v>
+        <v>4.012973378366607</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>46006.86041666667</v>
+        <v>46003.22152777778</v>
       </c>
       <c r="B10" t="n">
-        <v>-7.96</v>
+        <v>-7.98</v>
       </c>
       <c r="C10" t="n">
-        <v>114.15</v>
+        <v>114.18</v>
       </c>
       <c r="D10" t="n">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="E10" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="n">
-        <v>0.5</v>
+        <v>0.7823351233528767</v>
       </c>
       <c r="H10" t="n">
-        <v>50</v>
+        <v>78.23</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
+          <t>Terdampak</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>5.802792935549129</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>46003.22152777778</v>
+      </c>
+      <c r="B11" t="n">
+        <v>-7.98</v>
+      </c>
+      <c r="C11" t="n">
+        <v>114.18</v>
+      </c>
+      <c r="D11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E11" t="n">
+        <v>13</v>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="n">
+        <v>0.8780029949326082</v>
+      </c>
+      <c r="H11" t="n">
+        <v>87.8</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Terdampak</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>6.002316294436578</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>46003.23680555556</v>
+      </c>
+      <c r="B12" t="n">
+        <v>-7.97</v>
+      </c>
+      <c r="C12" t="n">
+        <v>114.13</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="E12" t="n">
+        <v>6</v>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="n">
+        <v>0.911968362286605</v>
+      </c>
+      <c r="H12" t="n">
+        <v>91.2</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Terdampak</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>4.057944861025488</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>46003.76111111111</v>
+      </c>
+      <c r="B13" t="n">
+        <v>-7.91</v>
+      </c>
+      <c r="C13" t="n">
+        <v>114.14</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" t="n">
+        <v>14</v>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="n">
+        <v>0.5636424251211228</v>
+      </c>
+      <c r="H13" t="n">
+        <v>56.36</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
           <t>Aman</t>
         </is>
       </c>
-      <c r="J10" t="n">
-        <v>4.113694388544492</v>
+      <c r="J13" t="n">
+        <v>3.156214049501883</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>46004.62708333333</v>
+      </c>
+      <c r="B14" t="n">
+        <v>-7.98</v>
+      </c>
+      <c r="C14" t="n">
+        <v>114.24</v>
+      </c>
+      <c r="D14" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="E14" t="n">
+        <v>10</v>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" t="n">
+        <v>100</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Terdampak</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>6.529222387025386</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>46004.62986111111</v>
+      </c>
+      <c r="B15" t="n">
+        <v>-7.99</v>
+      </c>
+      <c r="C15" t="n">
+        <v>114.21</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="E15" t="n">
+        <v>5</v>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="n">
+        <v>0.5371639818466017</v>
+      </c>
+      <c r="H15" t="n">
+        <v>53.72</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Aman</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>5.063326569954734</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>46004.62986111111</v>
+      </c>
+      <c r="B16" t="n">
+        <v>-7.99</v>
+      </c>
+      <c r="C16" t="n">
+        <v>114.21</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="E16" t="n">
+        <v>5</v>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="n">
+        <v>0.6581567157044004</v>
+      </c>
+      <c r="H16" t="n">
+        <v>65.81999999999999</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Aman</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>5.304787401220269</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>46004.97708333333</v>
+      </c>
+      <c r="B17" t="n">
+        <v>-7.99</v>
+      </c>
+      <c r="C17" t="n">
+        <v>114.22</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="E17" t="n">
+        <v>5</v>
+      </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="n">
+        <v>0.5146274993287281</v>
+      </c>
+      <c r="H17" t="n">
+        <v>51.46</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Aman</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>5.018351325334156</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>46004.97708333333</v>
+      </c>
+      <c r="B18" t="n">
+        <v>-7.99</v>
+      </c>
+      <c r="C18" t="n">
+        <v>114.22</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="E18" t="n">
+        <v>5</v>
+      </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="n">
+        <v>0.4953046286158333</v>
+      </c>
+      <c r="H18" t="n">
+        <v>49.53</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Aman</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>4.979789369785192</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>46004.99583333333</v>
+      </c>
+      <c r="B19" t="n">
+        <v>-7.97</v>
+      </c>
+      <c r="C19" t="n">
+        <v>114.16</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="E19" t="n">
+        <v>6</v>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="n">
+        <v>0.7863398500639497</v>
+      </c>
+      <c r="H19" t="n">
+        <v>78.63</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Terdampak</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>4.113867288164345</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>46006.00833333333</v>
+      </c>
+      <c r="B20" t="n">
+        <v>-7.97</v>
+      </c>
+      <c r="C20" t="n">
+        <v>114.15</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="E20" t="n">
+        <v>11</v>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="n">
+        <v>0.8449057463909231</v>
+      </c>
+      <c r="H20" t="n">
+        <v>84.48999999999999</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Terdampak</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>3.964490412458913</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>46006.48263888889</v>
+      </c>
+      <c r="B21" t="n">
+        <v>-7.99</v>
+      </c>
+      <c r="C21" t="n">
+        <v>114.19</v>
+      </c>
+      <c r="D21" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="E21" t="n">
+        <v>12</v>
+      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" t="n">
+        <v>100</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Terdampak</t>
+        </is>
+      </c>
+      <c r="J21" t="n">
+        <v>5.1946538276055</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>46006.86041666667</v>
+      </c>
+      <c r="B22" t="n">
+        <v>-7.96</v>
+      </c>
+      <c r="C22" t="n">
+        <v>114.15</v>
+      </c>
+      <c r="D22" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E22" t="n">
+        <v>10</v>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="n">
+        <v>0.8145592135071086</v>
+      </c>
+      <c r="H22" t="n">
+        <v>81.45999999999999</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Terdampak</t>
+        </is>
+      </c>
+      <c r="J22" t="n">
+        <v>4.631294577132157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>